<commit_message>
adjusted screws to match what was used
</commit_message>
<xml_diff>
--- a/hardware/Aaron Part List.xlsx
+++ b/hardware/Aaron Part List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhian\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhian\source\Aaron-Robot\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87609C5-D2C4-4B9C-8D7C-85E6F63BDD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0399724C-2909-4B1A-B601-748052F665E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{55B075A3-7C5D-48F4-BB65-04BCD371373F}"/>
+    <workbookView xWindow="3690" yWindow="3050" windowWidth="16920" windowHeight="11390" xr2:uid="{55B075A3-7C5D-48F4-BB65-04BCD371373F}"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanical" sheetId="1" r:id="rId1"/>
@@ -189,10 +189,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6D47C9-7D44-40DD-B585-15A7281A8545}">
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,71 +519,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="2:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -593,18 +593,21 @@
       </c>
       <c r="C3">
         <f>SUM(E3:I3) + J3*2 + K3*2 + L3*2 + M3*2 + N3*2 + O3*2 + P3*2 + Q3*2</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
       <c r="H3">
         <v>4</v>
       </c>
       <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
         <v>4</v>
       </c>
     </row>
@@ -632,6 +635,9 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J5">
         <v>4</v>
       </c>
       <c r="O5">
@@ -710,13 +716,19 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
       </c>
       <c r="E10">
         <v>4</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
       </c>
       <c r="H10">
         <v>4</v>
@@ -734,10 +746,16 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -933,20 +951,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C4EDF8-2A31-4933-9153-280CEBF4CDAF}">
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>